<commit_message>
remove duplicate in sorted array
</commit_message>
<xml_diff>
--- a/List of questions .xlsx
+++ b/List of questions .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\NamasteDSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE57D44A-7EC5-4552-87A8-C57DB9A2623F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CCB95D1-A387-4B3B-BCAD-360E09020268}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
   <si>
     <t>Print all even nos of an array</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>05_palindrome.js</t>
+  </si>
+  <si>
+    <t>Remove Duplicates from Sorted Array</t>
   </si>
 </sst>
 </file>
@@ -150,7 +153,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -164,6 +167,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -448,7 +452,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -613,10 +617,16 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="2"/>
-      <c r="B12" s="3"/>
+      <c r="A12" s="2">
+        <v>18</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>19</v>
+      </c>
       <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
+      <c r="D12" s="4">
+        <v>45858</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
@@ -672,6 +682,7 @@
     <hyperlink ref="C8" r:id="rId2" xr:uid="{14E8FDE0-F81B-4B72-90F7-C976F42CFC65}"/>
     <hyperlink ref="C10" r:id="rId3" display="Programming 101\05_palindrome.js" xr:uid="{43A3928B-CF65-4684-83E5-33271FE19537}"/>
     <hyperlink ref="C11" r:id="rId4" display="Programming 101\05_palindrome.js" xr:uid="{E1138DFE-F019-425E-B370-496A5DBD3C7C}"/>
+    <hyperlink ref="B12" r:id="rId5" display="https://leetcode.com/problems/remove-duplicates-from-sorted-array/" xr:uid="{5D4AFE06-6F7A-413E-800F-12CA9F0AD72B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
linked list delte from wnd
</commit_message>
<xml_diff>
--- a/List of questions .xlsx
+++ b/List of questions .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\NamasteDSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11295081-4D66-4F7E-95D1-C42A213951E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75FBDB52-7C22-494D-AF7A-EB23EE44489B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="87">
   <si>
     <t>Print all even nos of an array</t>
   </si>
@@ -277,6 +277,24 @@
   </si>
   <si>
     <t>Methods</t>
+  </si>
+  <si>
+    <t> Intersection of Two Linked Lists</t>
+  </si>
+  <si>
+    <t>04_Linked list\06_intersection.js</t>
+  </si>
+  <si>
+    <t>Remove Linked List Elements</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sentinel </t>
+  </si>
+  <si>
+    <t>Remove Nth Node From End of List</t>
+  </si>
+  <si>
+    <t>2 pointer</t>
   </si>
 </sst>
 </file>
@@ -328,7 +346,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -351,12 +369,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -374,11 +403,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -660,13 +691,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J38"/>
+  <dimension ref="A1:J41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B34" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B28" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B41" sqref="B41"/>
+      <selection pane="bottomRight" activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -680,34 +711,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="J1" s="9" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1608,16 +1639,85 @@
       <c r="F38" s="2">
         <v>2</v>
       </c>
-      <c r="G38" s="9" t="s">
+      <c r="G38" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H38" s="9">
+      <c r="H38" s="2">
         <v>234</v>
       </c>
       <c r="I38" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="J38" s="9" t="s">
+      <c r="J38" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A39" s="12">
+        <v>45</v>
+      </c>
+      <c r="B39" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="C39" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="D39" s="4">
+        <v>45900</v>
+      </c>
+      <c r="G39" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="H39" s="12">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A40" s="2">
+        <v>46</v>
+      </c>
+      <c r="B40" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="D40" s="13">
+        <v>45901</v>
+      </c>
+      <c r="E40" t="s">
+        <v>84</v>
+      </c>
+      <c r="H40" s="12">
+        <v>203</v>
+      </c>
+      <c r="J40" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A41" s="12">
+        <v>47</v>
+      </c>
+      <c r="B41" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="D41" s="13">
+        <v>45901</v>
+      </c>
+      <c r="E41" t="s">
+        <v>86</v>
+      </c>
+      <c r="F41">
+        <v>2</v>
+      </c>
+      <c r="G41" t="s">
+        <v>28</v>
+      </c>
+      <c r="H41" s="12">
+        <v>19</v>
+      </c>
+      <c r="I41" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="J41" s="2" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1671,8 +1771,12 @@
     <hyperlink ref="B38" r:id="rId46" display="https://leetcode.com/problems/palindrome-linked-list/" xr:uid="{FD127C40-A346-4931-B32E-AF83B61D8C73}"/>
     <hyperlink ref="C38" r:id="rId47" xr:uid="{00E15F8B-2C5F-4C2D-B5E8-899E26ED0C30}"/>
     <hyperlink ref="C37" r:id="rId48" xr:uid="{A76BCC80-6705-4B3C-BCE2-ADCBD9A14322}"/>
+    <hyperlink ref="B39" r:id="rId49" display="https://leetcode.com/problems/intersection-of-two-linked-lists/" xr:uid="{0505FF95-F86F-438C-AFE8-5129BA855EAB}"/>
+    <hyperlink ref="C39" r:id="rId50" xr:uid="{3FF4AACC-8542-499D-A2DE-BDE67DC9F496}"/>
+    <hyperlink ref="B40" r:id="rId51" display="https://leetcode.com/problems/remove-linked-list-elements/" xr:uid="{78D23C00-0B54-4D05-8414-348C8006E059}"/>
+    <hyperlink ref="B41" r:id="rId52" display="https://leetcode.com/problems/remove-nth-node-from-end-of-list/" xr:uid="{F161D37B-A8A9-46E4-93C2-3904B61DCAD3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId49"/>
+  <pageSetup orientation="portrait" r:id="rId53"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
inkeidn list  8 question
</commit_message>
<xml_diff>
--- a/List of questions .xlsx
+++ b/List of questions .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\NamasteDSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75FBDB52-7C22-494D-AF7A-EB23EE44489B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97DC3019-B81A-49B3-9733-E0CEA4B283DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="91">
   <si>
     <t>Print all even nos of an array</t>
   </si>
@@ -295,6 +295,18 @@
   </si>
   <si>
     <t>2 pointer</t>
+  </si>
+  <si>
+    <t>Remove Duplicates from Sorted List</t>
+  </si>
+  <si>
+    <t>Odd Even Linked List</t>
+  </si>
+  <si>
+    <t>Add Two Numbers</t>
+  </si>
+  <si>
+    <t>Merge Two Sorted Lists</t>
   </si>
 </sst>
 </file>
@@ -409,7 +421,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -691,13 +703,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J41"/>
+  <dimension ref="A1:J48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B28" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B44" sqref="B44"/>
+      <selection pane="bottomRight" activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1653,65 +1665,74 @@
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A39" s="12">
+      <c r="A39" s="2">
         <v>45</v>
       </c>
-      <c r="B39" s="11" t="s">
+      <c r="B39" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="C39" s="11" t="s">
+      <c r="C39" s="6" t="s">
         <v>82</v>
       </c>
       <c r="D39" s="4">
         <v>45900</v>
       </c>
-      <c r="G39" s="12" t="s">
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H39" s="12">
+      <c r="H39" s="2">
         <v>160</v>
       </c>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>46</v>
       </c>
-      <c r="B40" s="11" t="s">
+      <c r="B40" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="D40" s="13">
+      <c r="C40" s="2"/>
+      <c r="D40" s="4">
         <v>45901</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E40" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="H40" s="12">
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2">
         <v>203</v>
       </c>
-      <c r="J40" t="s">
+      <c r="I40" s="2"/>
+      <c r="J40" s="2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A41" s="12">
+      <c r="A41" s="2">
         <v>47</v>
       </c>
-      <c r="B41" s="11" t="s">
+      <c r="B41" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="D41" s="13">
+      <c r="C41" s="2"/>
+      <c r="D41" s="4">
         <v>45901</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E41" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="F41">
+      <c r="F41" s="2">
         <v>2</v>
       </c>
-      <c r="G41" t="s">
+      <c r="G41" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H41" s="12">
+      <c r="H41" s="2">
         <v>19</v>
       </c>
       <c r="I41" s="7" t="s">
@@ -1719,6 +1740,89 @@
       </c>
       <c r="J41" s="2" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A42" s="2">
+        <v>48</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C42" s="2"/>
+      <c r="D42" s="4">
+        <v>45901</v>
+      </c>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="13">
+        <v>83</v>
+      </c>
+      <c r="I42" s="2"/>
+      <c r="J42" s="2"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A43" s="2">
+        <v>49</v>
+      </c>
+      <c r="B43" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="D43" s="4">
+        <v>45901</v>
+      </c>
+      <c r="G43" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="H43" s="12">
+        <v>328</v>
+      </c>
+      <c r="I43" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A44" s="2">
+        <v>50</v>
+      </c>
+      <c r="B44" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D44" s="4">
+        <v>45901</v>
+      </c>
+      <c r="H44" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A45" s="2">
+        <v>51</v>
+      </c>
+      <c r="B45" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D45" s="4">
+        <v>45901</v>
+      </c>
+      <c r="H45">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A46" s="2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A47" s="2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A48" s="2">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1775,8 +1879,12 @@
     <hyperlink ref="C39" r:id="rId50" xr:uid="{3FF4AACC-8542-499D-A2DE-BDE67DC9F496}"/>
     <hyperlink ref="B40" r:id="rId51" display="https://leetcode.com/problems/remove-linked-list-elements/" xr:uid="{78D23C00-0B54-4D05-8414-348C8006E059}"/>
     <hyperlink ref="B41" r:id="rId52" display="https://leetcode.com/problems/remove-nth-node-from-end-of-list/" xr:uid="{F161D37B-A8A9-46E4-93C2-3904B61DCAD3}"/>
+    <hyperlink ref="B42" r:id="rId53" display="https://leetcode.com/problems/remove-duplicates-from-sorted-list/" xr:uid="{DF89E6B9-5554-47E2-BC3A-41024E45F6A5}"/>
+    <hyperlink ref="B43" r:id="rId54" display="https://leetcode.com/problems/odd-even-linked-list/" xr:uid="{623EDE4D-3916-45F4-AE7E-CD379E9022D0}"/>
+    <hyperlink ref="B44" r:id="rId55" display="https://leetcode.com/problems/add-two-numbers/" xr:uid="{F2F9ABCA-2B16-4EC8-B09A-7C3D4D34F24F}"/>
+    <hyperlink ref="B45" r:id="rId56" display="https://leetcode.com/problems/merge-two-sorted-lists/" xr:uid="{64A5FA11-C82E-4B19-A5CC-16EC9B08F4EB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId53"/>
+  <pageSetup orientation="portrait" r:id="rId57"/>
 </worksheet>
 </file>
</xml_diff>